<commit_message>
Censer files have been removed. Redundant code has been removed and everything has been consolidated into two files.
</commit_message>
<xml_diff>
--- a/ConfigFile/ConfigFile.xlsx
+++ b/ConfigFile/ConfigFile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Programacion\Documents\Robots\RPA Challenge\ConfigFile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E7481E2-B74B-4709-AE3C-5A63535345B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{979A40E5-4760-46F9-A0EE-915B44B8B680}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Agency</t>
   </si>
@@ -37,6 +37,18 @@
   </si>
   <si>
     <t>Agencies.xlsx</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>https://itdashboard.gov/</t>
+  </si>
+  <si>
+    <t>Directory Name</t>
+  </si>
+  <si>
+    <t>output</t>
   </si>
 </sst>
 </file>
@@ -366,12 +378,12 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -390,6 +402,23 @@
       <c r="B2" t="s">
         <v>3</v>
       </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="1"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E6" s="1"/>

</xml_diff>